<commit_message>
Fixed network and signature fail issues in DSL
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBRE22_Network.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBRE22_Network.xlsx
@@ -166,28 +166,6 @@
 };
 validate3
 {
-validate_Text_Exists=VT187-0750
-};
-validate4
-{
-validate_doesNotContain=Connected
-};
-validate5
-{
-validate_doesNotContain=Connected
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=RE 2.2 Tests
-};
-validate2
-{
-validate_PageTitle=Network
-};
-validate3
-{
 validate_Text_Exists=VT187-0757
 };
 validate4
@@ -216,6 +194,19 @@
 {
 validate_Result=Disconnected
 };</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(network22_test_link);
+wait(2);
+validate2;
+SelectTestToRun(VT187_0757_string);
+validate3;
+ClickRunTest(runtest_top_xpath);
+wait(5);
+validate4;
+press_Key(Home);</t>
   </si>
   <si>
     <t>wait(3);
@@ -234,7 +225,63 @@
 validate5;
 wifi_Mode(ON);
 wait(20);
-CheckUITextContains(Connected);
+press_Key(Home);</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(network22_test_link);
+wait(2);
+validate2;
+SelectTestToRun(VT187_0751_string);
+validate3;
+ClickRunTest(runtest_top_xpath);
+validate4;
+wifi_Mode(OFF);
+wait(2);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+validate5;
+wifi_Mode(ON);
+wait(20);
+press_Key(Home);</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(network22_test_link);
+wait(2);
+validate2;
+SelectTestToRun(VT187_0755_string);
+validate3;
+ClickRunTest(runtest_top_xpath);
+validate4;
+wifi_Mode(OFF);
+wait(60);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+validate5;
+wifi_Mode(ON);
+wait(20);
+press_Key(Home);</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(network22_test_link);
+wait(2);
+validate2;
+SelectTestToRun(VT187_0752_string);
+validate3;
+ClickRunTest(runtest_top_xpath);
+validate4;
+wifi_Mode(OFF);
+wait(2);
+press_Key(Home);
+launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
+validate5;
+wifi_Mode(ON);
+wait(20);
 press_Key(Home);</t>
   </si>
   <si>
@@ -254,81 +301,29 @@
 validate5;
 wifi_Mode(ON);
 wait(20);
-CheckUITextContains(Connected);
 press_Key(Home);</t>
   </si>
   <si>
-    <t>wait(3);
-validate1;
-link_Click(network22_test_link);
-wait(2);
-validate2;
-SelectTestToRun(VT187_0751_string);
-validate3;
-ClickRunTest(runtest_top_xpath);
-validate4;
-wifi_Mode(OFF);
-wait(2);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-validate5;
-wifi_Mode(ON);
-wait(20);
-CheckUITextContains(Connected);
-press_Key(Home);</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(network22_test_link);
-wait(2);
-validate2;
-SelectTestToRun(VT187_0752_string);
-validate3;
-ClickRunTest(runtest_top_xpath);
-validate4;
-wifi_Mode(OFF);
-wait(2);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-validate5;
-wifi_Mode(ON);
-wait(20);
-CheckUITextContains(Connected);
-press_Key(Home);</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(network22_test_link);
-wait(2);
-validate2;
-SelectTestToRun(VT187_0755_string);
-validate3;
-ClickRunTest(runtest_top_xpath);
-validate4;
-wifi_Mode(OFF);
-wait(60);
-press_Key(Home);
-launch_App_Device(com.symbol.enterprisebrowser/com.rhomobile.rhodes.RhodesActivity);
-validate5;
-wifi_Mode(ON);
-wait(20);
-CheckUITextContains(Connected);
-press_Key(Home);</t>
-  </si>
-  <si>
-    <t>wait(3);
-validate1;
-link_Click(network22_test_link);
-wait(2);
-validate2;
-SelectTestToRun(VT187_0757_string);
-validate3;
-ClickRunTest(runtest_top_xpath);
-wait(5);
-validate4;
-press_Key(Home);</t>
+    <t>validate1
+{
+validate_PageTitle=RE 2.2 Tests
+};
+validate2
+{
+validate_PageTitle=Network
+};
+validate3
+{
+validate_Text_Exists=VT187-0750
+};
+validate4
+{
+validate_Result=Connected
+};
+validate5
+{
+validate_doesNotContain=Disconnected
+};</t>
   </si>
 </sst>
 </file>
@@ -832,7 +827,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -951,10 +946,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -978,7 +973,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H5" s="11" t="s">
         <v>21</v>
@@ -1032,10 +1027,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -1048,7 +1043,7 @@
       <c r="B8" s="15">
         <v>1</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E8" s="14" t="s">
@@ -1058,10 +1053,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>